<commit_message>
update fvplans - clean-up
remove verification items not implemented in cv32e40p
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/FormalVerificationPlan/base_instruction_set/CV32E40P_RV32C_Extension_Instructions.xlsx
+++ b/verif/CV32E40P/FormalVerificationPlan/base_instruction_set/CV32E40P_RV32C_Extension_Instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\salah\Documents\OneSpin\Work\RISC-V\OpenHW\core_v_doc\core-v-docs-formal_vplan\verif\CV32E40P\FormalVerificationPlan\base_instruction_set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntusinschi\Dropbox\OpenHW-Project\forkHW\core-v-docs\verif\CV32E40P\FormalVerificationPlan\base_instruction_set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37435776-3115-4D79-901D-6BE7E9039210}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11769381-29FB-48CD-A748-894C53378D78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RVC" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="106">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>Link to Coverage</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- END -----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------</t>
   </si>
   <si>
     <t>Self Checking Test</t>
@@ -245,72 +242,6 @@
     </r>
   </si>
   <si>
-    <t>C.FLWSP
-(RV32FC)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>c.flwsp rd, uimm(x2)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-f[rd] = M[x[2] + uimm][0:31]
-Expands to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>flw rd, uimm[7:2](x2)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.
-uimm treated as </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-      </rPr>
-      <t>unsigned</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> number</t>
-    </r>
-  </si>
-  <si>
     <t>C.SWSP</t>
   </si>
   <si>
@@ -376,72 +307,6 @@
     </r>
   </si>
   <si>
-    <t>C.FSWSP
-(RV32FC)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>c.fswsp rs2, uimm(x2)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-M[x[2] + uimm][0:31] = f[rs2]
-Expands to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>fsw rs2, offset[7:2](x2)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">.
-uimm treated as </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-      </rPr>
-      <t>unsigned</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> number</t>
-    </r>
-  </si>
-  <si>
     <t>C.LW</t>
   </si>
   <si>
@@ -477,52 +342,6 @@
     </r>
   </si>
   <si>
-    <t>C.FLW
-(RV32FC)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>c.flw rd', uimm(rs1')</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-f[rd] = M[x[rs1] + uimm][0:31], where rd=8+rd' and rs1=8+rs1'
-Expands to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>flw rd', uimm[6:2](rs1')</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>C.SW</t>
   </si>
   <si>
@@ -555,52 +374,6 @@
         <family val="3"/>
       </rPr>
       <t>sw rs2', uimm[6:2](rs1')</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <t>C.FSW
-(RV32FC)</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>c.fsw rs2', uimm(rs1')</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-M[x[rs1] + uimm][0:31] = f[rs2], where rs2=8+rs2' and rs1=8+rs1'
-Expands to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>fsw rs2', uimm[6:2](rs1')</t>
     </r>
     <r>
       <rPr>
@@ -1738,18 +1511,6 @@
   </si>
   <si>
     <t>Normal instruction with rd=x0, rs2≠0</t>
-  </si>
-  <si>
-    <t>C.SLLI64</t>
-  </si>
-  <si>
-    <t>Normal instruction with nzimm=0</t>
-  </si>
-  <si>
-    <t>C.SRLI64</t>
-  </si>
-  <si>
-    <t>C.SRAI64</t>
   </si>
   <si>
     <t>RVC
@@ -1883,7 +1644,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1892,13 +1653,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFAFF0AF"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1915,7 +1670,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1925,12 +1680,6 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1970,24 +1719,25 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2372,28 +2122,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMM43"/>
+  <dimension ref="A1:AMM35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" activeCellId="4" sqref="A40:XFD42 A3:XFD3 A5:XFD5 A7:XFD7 A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="75.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.88671875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="75.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="64.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.88671875" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="1025" width="17" style="1" customWidth="1"/>
-    <col min="1026" max="1027" width="9.140625" style="1" customWidth="1"/>
+    <col min="1026" max="1027" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1">
@@ -2413,1337 +2163,1104 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>24</v>
+      <c r="J1" s="23" t="s">
+        <v>23</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="74.25">
+    <row r="2" spans="1:11" s="4" customFormat="1" ht="70.2">
       <c r="A2" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K2" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F2" s="12" t="s">
+      <c r="D3" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" s="13" t="s">
+      <c r="F3" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="4" customFormat="1" ht="42.6">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="F4" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="4" customFormat="1" ht="42.6">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="59.25">
-      <c r="A3" s="25"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="26" t="s">
-        <v>43</v>
-      </c>
-      <c r="D3" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F3" s="12" t="s">
+      <c r="F5" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A6" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="E6" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="13" t="s">
+      <c r="F6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="4" customFormat="1" ht="42">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="13" t="s">
+      <c r="F7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J7" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="4" customFormat="1" ht="42.6">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="59.25">
-      <c r="A4" s="25"/>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="12" t="s">
+      <c r="F8" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="4" customFormat="1" ht="42.6">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="E9" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J4" s="13" t="s">
+      <c r="F9" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="13" t="s">
+      <c r="F10" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="59.25">
-      <c r="A5" s="25"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F5" s="12" t="s">
+      <c r="F11" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A12" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J5" s="13" t="s">
+      <c r="F12" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="E13" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="F13" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="17" customFormat="1" ht="70.2">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="E14" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A6" s="25"/>
-      <c r="B6" s="21"/>
-      <c r="C6" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="D6" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" s="12" t="s">
+      <c r="F14" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="I14" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K14" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D15" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="E15" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J6" s="13" t="s">
+      <c r="F15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K6" s="13" t="s">
+      <c r="F16" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A7" s="25"/>
-      <c r="B7" s="21"/>
-      <c r="C7" s="26" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="E7" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="F17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J17" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K17" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="4" customFormat="1" ht="58.8">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E18" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J7" s="13" t="s">
+      <c r="F18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="4" customFormat="1" ht="45">
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E19" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="13" t="s">
+      <c r="F19" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E20" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A8" s="25"/>
-      <c r="B8" s="21"/>
-      <c r="C8" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="D8" s="20" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F8" s="12" t="s">
+      <c r="F20" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K20" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="4" customFormat="1" ht="42.6">
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D21" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="E21" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="13" t="s">
+      <c r="F21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K21" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="4" customFormat="1" ht="56.4">
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+      <c r="C22" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="E22" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K8" s="13" t="s">
+      <c r="F22" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="4" customFormat="1" ht="42.6">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="21"/>
-      <c r="C9" s="26" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="12" t="s">
+      <c r="F23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="4" customFormat="1" ht="42.6">
+      <c r="A24" s="25"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="E24" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I9" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J9" s="13" t="s">
+      <c r="F24" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K24" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="4" customFormat="1" ht="42.6">
+      <c r="A25" s="25"/>
+      <c r="B25" s="26"/>
+      <c r="C25" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K9" s="13" t="s">
+      <c r="F25" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="4" customFormat="1" ht="42.6">
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="18" t="s">
+        <v>89</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="16" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="58.5">
-      <c r="A10" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F10" s="12" t="s">
+      <c r="F26" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J26" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K26" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="4" customFormat="1" ht="41.4">
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E27" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J10" s="13" t="s">
+      <c r="F27" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K27" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" s="4" customFormat="1" ht="42.6">
+      <c r="A28" s="25"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="13" t="s">
+      <c r="F28" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J28" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" s="4" customFormat="1" ht="41.4">
+      <c r="A29" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="43.5">
-      <c r="A11" s="25"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F11" s="12" t="s">
+      <c r="F29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="4" customFormat="1" ht="41.4">
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E30" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J11" s="13" t="s">
+      <c r="F30" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K30" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="4" customFormat="1" ht="41.4">
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="K11" s="13" t="s">
+      <c r="F31" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J31" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K31" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="4" customFormat="1" ht="41.4">
+      <c r="A32" s="25"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E32" s="20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="21"/>
-      <c r="C12" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="D12" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="12" t="s">
+      <c r="F32" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" s="4" customFormat="1" ht="41.4">
+      <c r="A33" s="25"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E33" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J12" s="13" t="s">
+      <c r="F33" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J33" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" s="4" customFormat="1" ht="41.4">
+      <c r="A34" s="25"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E34" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="K12" s="13" t="s">
+      <c r="F34" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J34" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" s="4" customFormat="1" ht="41.4">
+      <c r="A35" s="25"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="21"/>
-      <c r="C13" s="20" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F13" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I13" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K13" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="4" customFormat="1" ht="58.5">
-      <c r="A14" s="25"/>
-      <c r="B14" s="21"/>
-      <c r="C14" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="E14" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="58.5">
-      <c r="A15" s="25"/>
-      <c r="B15" s="21"/>
-      <c r="C15" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K15" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="58.5">
-      <c r="A16" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K16" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="58.5">
-      <c r="A17" s="25"/>
-      <c r="B17" s="21"/>
-      <c r="C17" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J17" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="19" customFormat="1" ht="72.75">
-      <c r="A18" s="25"/>
-      <c r="B18" s="21"/>
-      <c r="C18" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="E18" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="J18" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="4" customFormat="1" ht="58.5">
-      <c r="A19" s="25"/>
-      <c r="B19" s="21"/>
-      <c r="C19" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D19" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J19" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K19" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" ht="58.5">
-      <c r="A20" s="25"/>
-      <c r="B20" s="21"/>
-      <c r="C20" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J20" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K20" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="58.5">
-      <c r="A21" s="25"/>
-      <c r="B21" s="21"/>
-      <c r="C21" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D21" s="20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E21" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F21" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I21" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J21" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K21" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="63">
-      <c r="A22" s="25"/>
-      <c r="B22" s="21"/>
-      <c r="C22" s="20" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E22" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F22" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J22" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K22" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="48.75">
-      <c r="A23" s="25"/>
-      <c r="B23" s="21"/>
-      <c r="C23" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F23" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G23" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I23" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" ht="59.25">
-      <c r="A24" s="25"/>
-      <c r="B24" s="21"/>
-      <c r="C24" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="D24" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="E24" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F24" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I24" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J24" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K24" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A25" s="25"/>
-      <c r="B25" s="21"/>
-      <c r="C25" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D25" s="20" t="s">
-        <v>90</v>
-      </c>
-      <c r="E25" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H25" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I25" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J25" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" ht="58.5">
-      <c r="A26" s="25"/>
-      <c r="B26" s="21"/>
-      <c r="C26" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>118</v>
-      </c>
-      <c r="E26" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G26" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I26" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K26" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A27" s="25"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I27" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J27" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K27" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="21"/>
-      <c r="C28" s="20" t="s">
-        <v>94</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="E28" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G28" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J28" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K28" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A29" s="25"/>
-      <c r="B29" s="21"/>
-      <c r="C29" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="E29" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I29" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J29" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K29" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A30" s="25"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="20" t="s">
-        <v>98</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="E30" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G30" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H30" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I30" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J30" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K30" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A31" s="25"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>101</v>
-      </c>
-      <c r="E31" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F31" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G31" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H31" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I31" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K31" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" ht="44.25">
-      <c r="A32" s="25"/>
-      <c r="B32" s="21"/>
-      <c r="C32" s="20" t="s">
-        <v>102</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="E32" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G32" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I32" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J32" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K32" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A33" s="25" t="s">
-        <v>104</v>
-      </c>
-      <c r="B33" s="21" t="s">
-        <v>117</v>
-      </c>
-      <c r="C33" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="D33" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="E33" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F33" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G33" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I33" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J33" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K33" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A34" s="25"/>
-      <c r="B34" s="21"/>
-      <c r="C34" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="D34" s="23" t="s">
-        <v>106</v>
-      </c>
-      <c r="E34" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F34" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G34" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H34" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I34" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J34" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K34" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A35" s="25"/>
-      <c r="B35" s="21"/>
-      <c r="C35" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="D35" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="E35" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F35" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G35" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H35" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I35" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J35" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K35" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A36" s="25"/>
-      <c r="B36" s="21"/>
-      <c r="C36" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D36" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="E36" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F36" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G36" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H36" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J36" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K36" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A37" s="25"/>
-      <c r="B37" s="21"/>
-      <c r="C37" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="D37" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E37" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F37" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I37" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J37" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K37" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A38" s="25"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E38" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H38" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I38" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J38" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K38" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A39" s="25"/>
-      <c r="B39" s="21"/>
-      <c r="C39" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="D39" s="23" t="s">
-        <v>108</v>
-      </c>
-      <c r="E39" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F39" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G39" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H39" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I39" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J39" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K39" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A40" s="25"/>
-      <c r="B40" s="21"/>
-      <c r="C40" s="20" t="s">
-        <v>110</v>
-      </c>
-      <c r="D40" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F40" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G40" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H40" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I40" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J40" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K40" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A41" s="25"/>
-      <c r="B41" s="21"/>
-      <c r="C41" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="D41" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="E41" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F41" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G41" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H41" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I41" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J41" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K41" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" s="4" customFormat="1" ht="42.75">
-      <c r="A42" s="25"/>
-      <c r="B42" s="21"/>
-      <c r="C42" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="F42" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="G42" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H42" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I42" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="J42" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="K42" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" s="5" customFormat="1">
-      <c r="A43" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="B43" s="22"/>
-      <c r="C43" s="22"/>
-      <c r="D43" s="22"/>
-      <c r="E43" s="22"/>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-      <c r="J43" s="22"/>
-      <c r="K43" s="6"/>
+      <c r="F35" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" s="11" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="A2:A9"/>
-    <mergeCell ref="B2:B9"/>
-    <mergeCell ref="A10:A15"/>
-    <mergeCell ref="B10:B15"/>
-    <mergeCell ref="A16:A32"/>
-    <mergeCell ref="B16:B32"/>
-    <mergeCell ref="A33:A42"/>
-    <mergeCell ref="B33:B42"/>
-    <mergeCell ref="A43:J43"/>
+  <mergeCells count="8">
+    <mergeCell ref="A29:A35"/>
+    <mergeCell ref="B29:B35"/>
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="A6:A11"/>
+    <mergeCell ref="B6:B11"/>
+    <mergeCell ref="A12:A28"/>
+    <mergeCell ref="B12:B28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -3754,25 +3271,25 @@
           <x14:formula1>
             <xm:f>DONOTDELETE!$A$3:$A$55</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F42</xm:sqref>
+          <xm:sqref>F2:F35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DDDA95CE-2B91-4BF6-A07B-87518765EC90}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$C$3:$C$8</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G42</xm:sqref>
+          <xm:sqref>G2:G35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C1B4F20-53D1-4A1B-832B-6E8BECAAA5F1}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$E$3:$E$8</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H42</xm:sqref>
+          <xm:sqref>H2:H35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79222D68-7559-4143-9FDD-D11E5D5A8DF0}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$G$3:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I42</xm:sqref>
+          <xm:sqref>I2:I35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3788,140 +3305,140 @@
       <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="2.85546875" customWidth="1"/>
+    <col min="2" max="2" width="2.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2.88671875" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
-      <c r="A2" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="11" t="s">
+      <c r="A2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11" t="s">
+      <c r="D2" s="9"/>
+      <c r="E2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Annotate OneSpin FV Results
Populate the plans w/ tests and results
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/FormalVerificationPlan/base_instruction_set/CV32E40P_RV32C_Extension_Instructions.xlsx
+++ b/verif/CV32E40P/FormalVerificationPlan/base_instruction_set/CV32E40P_RV32C_Extension_Instructions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ntusinschi\Dropbox\OpenHW-Project\forkHW\core-v-docs\verif\CV32E40P\FormalVerificationPlan\base_instruction_set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11769381-29FB-48CD-A748-894C53378D78}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4055F18-BCE9-4A70-8BD5-D7CDD50FD6EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="94">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Check against RM</t>
   </si>
   <si>
-    <t>Other</t>
-  </si>
-  <si>
     <t>Assertion Check</t>
   </si>
   <si>
@@ -90,61 +87,10 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Full Proof</t>
-  </si>
-  <si>
-    <t>Witness</t>
-  </si>
-  <si>
     <t>Observation Coverage</t>
   </si>
   <si>
-    <t>Partial Proof</t>
-  </si>
-  <si>
     <t>Properties</t>
-  </si>
-  <si>
-    <t>Coverage Details</t>
-  </si>
-  <si>
-    <t>RV32I.Arith_a</t>
-  </si>
-  <si>
-    <t>RV32I.Mem_a</t>
-  </si>
-  <si>
-    <t>RV32I.Branch_a</t>
-  </si>
-  <si>
-    <t>RV32I.Jump_a</t>
-  </si>
-  <si>
-    <t>RVC.Arith_a</t>
-  </si>
-  <si>
-    <t>RVC.Branch_a</t>
-  </si>
-  <si>
-    <t>RVC.Jump_a</t>
-  </si>
-  <si>
-    <t>RVC.Mem_a</t>
-  </si>
-  <si>
-    <t>RV32M.all_a</t>
-  </si>
-  <si>
-    <t>RV32I.CSR_a</t>
-  </si>
-  <si>
-    <t>RV32I.Ret_a</t>
-  </si>
-  <si>
-    <t>RV32I.CallBreak_a</t>
-  </si>
-  <si>
-    <t>RV32I.FENCE_a</t>
   </si>
   <si>
     <t>TBD</t>
@@ -1407,51 +1353,6 @@
     </r>
   </si>
   <si>
-    <t>C.EBREAK</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>c.ebreak</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">
-RaiseException(Breakpoint)
-Expands to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Courier New"/>
-        <family val="3"/>
-      </rPr>
-      <t>ebreak</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="DejaVu Sans"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
     <t>Unprivileged ISA
 Chapter 16.7</t>
   </si>
@@ -1570,6 +1471,30 @@
       <t>. Invalid when rd=x0 or rs2=x0.
 Arithmetic overflow is ignored</t>
     </r>
+  </si>
+  <si>
+    <t>RV_chk.ops.RVC.Arith_a</t>
+  </si>
+  <si>
+    <t>RV_chk.ops.RVC.Jump_a</t>
+  </si>
+  <si>
+    <t>Partial Proof w/ Reachable Witness</t>
+  </si>
+  <si>
+    <t>Full Proof w/ Reachable Witness</t>
+  </si>
+  <si>
+    <t>Reachable Witness</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>RV_chk.ops.RVC.Mem_*a</t>
+  </si>
+  <si>
+    <t>RV_chk.ops.RVC.Branch_*a</t>
   </si>
 </sst>
 </file>
@@ -1653,7 +1578,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1670,7 +1595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1699,14 +1624,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1727,18 +1646,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2122,11 +2037,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMM35"/>
+  <dimension ref="A1:AML35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" activeCellId="4" sqref="A40:XFD42 A3:XFD3 A5:XFD5 A7:XFD7 A9:XFD9"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2136,17 +2051,16 @@
     <col min="3" max="3" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="75.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="64.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="1025" width="17" style="1" customWidth="1"/>
-    <col min="1026" max="1027" width="9.109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="33.21875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="21.109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="27.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="1024" width="17" style="1" customWidth="1"/>
+    <col min="1025" max="1026" width="9.109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1">
+    <row r="1" spans="1:10" s="4" customFormat="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2163,1133 +2077,1012 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" ht="70.2">
+      <c r="A2" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" s="4" customFormat="1" ht="70.2">
-      <c r="A2" s="25" t="s">
+      <c r="E2" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J2" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A3" s="20"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J3" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" s="4" customFormat="1" ht="42.6">
+      <c r="A4" s="20"/>
+      <c r="B4" s="21"/>
+      <c r="C4" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" s="4" customFormat="1" ht="42.6">
+      <c r="A5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A6" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="4" customFormat="1" ht="42">
+      <c r="A7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="42.6">
+      <c r="A8" s="20"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" s="4" customFormat="1" ht="42.6">
+      <c r="A9" s="20"/>
+      <c r="B9" s="21"/>
+      <c r="C9" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C2" s="18" t="s">
+      <c r="D10" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="18" t="s">
+      <c r="E10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A11" s="20"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
-      <c r="C3" s="18" t="s">
+      <c r="D11" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="E11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J11" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A12" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" s="4" customFormat="1" ht="42.6">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="18" t="s">
+      <c r="B12" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D12" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" s="4" customFormat="1" ht="42.6">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
-      <c r="C5" s="18" t="s">
+      <c r="E12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J12" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D13" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A6" s="25" t="s">
+      <c r="E13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J13" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="15" customFormat="1" ht="70.2">
+      <c r="A14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="C6" s="18" t="s">
+      <c r="D14" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E14" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="E6" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H6" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J6" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" s="4" customFormat="1" ht="42">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="18" t="s">
+      <c r="D15" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D7" s="18" t="s">
+      <c r="E15" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J15" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A16" s="20"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" s="4" customFormat="1" ht="42.6">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="18" t="s">
+      <c r="D16" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="E16" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A17" s="20"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J8" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" s="4" customFormat="1" ht="42.6">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="18" t="s">
+      <c r="D17" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="E17" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J17" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" s="4" customFormat="1" ht="58.8">
+      <c r="A18" s="20"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="E9" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I9" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K9" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="18" t="s">
+      <c r="D18" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="E18" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J18" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="4" customFormat="1" ht="45">
+      <c r="A19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I10" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J10" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K10" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A11" s="25"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="18" t="s">
+      <c r="D19" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="D11" s="18" t="s">
+      <c r="E19" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J19" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J11" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K11" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A12" s="25" t="s">
+      <c r="D20" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B12" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="C12" s="18" t="s">
+      <c r="E20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J20" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="4" customFormat="1" ht="42.6">
+      <c r="A21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D21" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="E12" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J12" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="18" t="s">
+      <c r="E21" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J21" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="4" customFormat="1" ht="56.4">
+      <c r="A22" s="20"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D22" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" s="4" customFormat="1" ht="42.6">
+      <c r="A23" s="20"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E13" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J13" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" s="17" customFormat="1" ht="70.2">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="18" t="s">
+      <c r="D23" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="E23" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J23" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" s="4" customFormat="1" ht="42.6">
+      <c r="A24" s="20"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="G14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="18" t="s">
+      <c r="D24" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="E24" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J24" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" s="4" customFormat="1" ht="42.6">
+      <c r="A25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I15" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K15" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="18" t="s">
+      <c r="D25" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="E25" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J25" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" s="4" customFormat="1" ht="42.6">
+      <c r="A26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K16" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A17" s="25"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="18" t="s">
+      <c r="D26" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="E26" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J26" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" s="4" customFormat="1" ht="41.4">
+      <c r="A27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J17" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K17" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" s="4" customFormat="1" ht="58.8">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="18" t="s">
+      <c r="D27" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="D18" s="18" t="s">
+      <c r="E27" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J27" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="4" customFormat="1" ht="41.4">
+      <c r="A28" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J18" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K18" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" s="4" customFormat="1" ht="45">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="18" t="s">
+      <c r="B28" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" s="17" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="E28" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="41.4">
+      <c r="A29" s="20"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H19" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J19" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K19" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="18" t="s">
+      <c r="E29" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J29" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" s="4" customFormat="1" ht="41.4">
+      <c r="A30" s="20"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="18" t="s">
+      <c r="E30" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" s="4" customFormat="1" ht="41.4">
+      <c r="A31" s="20"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D31" s="17" t="s">
         <v>79</v>
       </c>
-      <c r="E20" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J20" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K20" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" s="4" customFormat="1" ht="42.6">
-      <c r="A21" s="25"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="18" t="s">
+      <c r="E31" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" s="4" customFormat="1" ht="41.4">
+      <c r="A32" s="20"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D32" s="17" t="s">
         <v>80</v>
       </c>
-      <c r="D21" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="E21" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H21" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J21" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K21" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" s="4" customFormat="1" ht="56.4">
-      <c r="A22" s="25"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D22" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="E22" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H22" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K22" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="4" customFormat="1" ht="42.6">
-      <c r="A23" s="25"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H23" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J23" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K23" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" s="4" customFormat="1" ht="42.6">
-      <c r="A24" s="25"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="18" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="18" t="s">
+      <c r="E32" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F24" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J24" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K24" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" s="4" customFormat="1" ht="42.6">
-      <c r="A25" s="25"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="D25" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J25" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K25" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" s="4" customFormat="1" ht="42.6">
-      <c r="A26" s="25"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="18" t="s">
-        <v>89</v>
-      </c>
-      <c r="D26" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H26" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J26" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K26" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" s="4" customFormat="1" ht="41.4">
-      <c r="A27" s="25"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="18" t="s">
+      <c r="G32" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H32" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J32" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D27" s="18" t="s">
-        <v>92</v>
-      </c>
-      <c r="E27" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J27" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K27" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" s="4" customFormat="1" ht="42.6">
-      <c r="A28" s="25"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="18" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="E28" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F28" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G28" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H28" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J28" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K28" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" s="4" customFormat="1" ht="41.4">
-      <c r="A29" s="25" t="s">
-        <v>95</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="C29" s="18" t="s">
+    </row>
+    <row r="33" spans="1:10" s="4" customFormat="1" ht="41.4">
+      <c r="A33" s="20"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D33" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="E33" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="I33" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="J33" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="D29" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="E29" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J29" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K29" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="4" customFormat="1" ht="41.4">
-      <c r="A30" s="25"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="D30" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="E30" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J30" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="4" customFormat="1" ht="41.4">
-      <c r="A31" s="25"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="D31" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="E31" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F31" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H31" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I31" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J31" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="4" customFormat="1" ht="41.4">
-      <c r="A32" s="25"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="D32" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E32" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H32" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I32" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J32" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" ht="41.4">
-      <c r="A33" s="25"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D33" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E33" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G33" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H33" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I33" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J33" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" s="4" customFormat="1" ht="41.4">
-      <c r="A34" s="25"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="E34" s="20" t="s">
-        <v>38</v>
+    </row>
+    <row r="34" spans="1:10" s="4" customFormat="1" ht="41.4">
+      <c r="A34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="E34" s="18" t="s">
+        <v>20</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>37</v>
+        <v>86</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H34" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I34" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J34" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="4" customFormat="1" ht="41.4">
-      <c r="A35" s="25"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="D35" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E35" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="H35" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J35" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="K35" s="11" t="s">
-        <v>37</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10">
+      <c r="A35" s="22"/>
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="A29:A35"/>
-    <mergeCell ref="B29:B35"/>
+    <mergeCell ref="A28:A34"/>
+    <mergeCell ref="B28:B34"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="A6:A11"/>
     <mergeCell ref="B6:B11"/>
-    <mergeCell ref="A12:A28"/>
-    <mergeCell ref="B12:B28"/>
+    <mergeCell ref="A12:A27"/>
+    <mergeCell ref="B12:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E241BCDD-D334-4632-B093-6E0F954103AD}">
-          <x14:formula1>
-            <xm:f>DONOTDELETE!$A$3:$A$55</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F35</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DDDA95CE-2B91-4BF6-A07B-87518765EC90}">
-          <x14:formula1>
-            <xm:f>DONOTDELETE!$C$3:$C$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>G2:G35</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C1B4F20-53D1-4A1B-832B-6E8BECAAA5F1}">
-          <x14:formula1>
-            <xm:f>DONOTDELETE!$E$3:$E$8</xm:f>
-          </x14:formula1>
-          <xm:sqref>H2:H35</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{79222D68-7559-4143-9FDD-D11E5D5A8DF0}">
           <x14:formula1>
             <xm:f>DONOTDELETE!$G$3:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I35</xm:sqref>
+          <xm:sqref>I2:I34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DDDA95CE-2B91-4BF6-A07B-87518765EC90}">
+          <x14:formula1>
+            <xm:f>DONOTDELETE!$C$3:$C$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>G2:G34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C1B4F20-53D1-4A1B-832B-6E8BECAAA5F1}">
+          <x14:formula1>
+            <xm:f>DONOTDELETE!$E$3:$E$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>H2:H34</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E241BCDD-D334-4632-B093-6E0F954103AD}">
+          <x14:formula1>
+            <xm:f>DONOTDELETE!$A$3:$A$52</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F34</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3299,33 +3092,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F715C8E-197B-44C9-9B60-317E26D89669}">
-  <dimension ref="A2:G16"/>
+  <dimension ref="A2:G7"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+      <selection activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="2.88671875" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="2.88671875" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="2.88671875" customWidth="1"/>
-    <col min="7" max="7" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="9"/>
       <c r="E2" s="9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="9"/>
       <c r="G2" s="9" t="s">
@@ -3334,111 +3127,63 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>92</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>